<commit_message>
update documentation and pinmap
</commit_message>
<xml_diff>
--- a/pinmap/pinmaps.xlsx
+++ b/pinmap/pinmaps.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88A8B434-129D-C449-BFCA-955245AD3DC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FE08CCC-3413-4CB4-9DF2-C9C66431A9B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="18600" windowHeight="15980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5130" yWindow="150" windowWidth="19515" windowHeight="15210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pinouts" sheetId="3" r:id="rId1"/>
@@ -446,7 +446,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-DE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -537,7 +537,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="en-DE"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -729,7 +729,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-DE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="401323392"/>
@@ -791,7 +791,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-DE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="401317488"/>
@@ -832,7 +832,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="en-DE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -883,7 +883,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-DE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -974,7 +974,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="en-DE"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1178,7 +1178,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-DE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="532417304"/>
@@ -1240,7 +1240,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-DE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="532421240"/>
@@ -1281,7 +1281,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="en-DE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2752,21 +2752,21 @@
   <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" customWidth="1"/>
-    <col min="2" max="2" width="47.6640625" customWidth="1"/>
-    <col min="3" max="5" width="7.33203125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="7.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="3.33203125" customWidth="1"/>
-    <col min="8" max="8" width="7.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="7.33203125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="2" max="2" width="67.28515625" customWidth="1"/>
+    <col min="3" max="5" width="7.28515625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="7.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.28515625" customWidth="1"/>
+    <col min="8" max="8" width="7.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="7.28515625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -2795,7 +2795,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2827,7 +2827,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -2859,7 +2859,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -2891,7 +2891,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -2923,7 +2923,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D6" s="3" t="s">
         <v>81</v>
       </c>
@@ -2946,7 +2946,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C7" s="3" t="s">
         <v>21</v>
       </c>
@@ -2972,7 +2972,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C8" s="3" t="s">
         <v>22</v>
       </c>
@@ -2998,7 +2998,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C9" s="3" t="s">
         <v>23</v>
       </c>
@@ -3024,7 +3024,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C10" s="3" t="s">
         <v>24</v>
       </c>
@@ -3050,7 +3050,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C11" s="6" t="s">
         <v>20</v>
       </c>
@@ -3076,7 +3076,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C12" s="6" t="s">
         <v>20</v>
       </c>
@@ -3102,7 +3102,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C13" s="5" t="s">
         <v>27</v>
       </c>
@@ -3128,7 +3128,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D14" s="3" t="s">
         <v>57</v>
       </c>
@@ -3140,7 +3140,7 @@
       </c>
       <c r="H14" s="4"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D15" s="3" t="s">
         <v>58</v>
       </c>
@@ -3152,7 +3152,7 @@
       </c>
       <c r="H15" s="4"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D16" s="3" t="s">
         <v>59</v>
       </c>
@@ -3164,7 +3164,7 @@
       </c>
       <c r="H16" s="4"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C18" s="3" t="s">
         <v>19</v>
       </c>
@@ -3187,7 +3187,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B20" s="7" t="s">
         <v>39</v>
       </c>
@@ -3204,7 +3204,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C21" s="3" t="s">
         <v>51</v>
       </c>
@@ -3218,7 +3218,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C22" s="3" t="s">
         <v>50</v>
       </c>
@@ -3232,7 +3232,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C23" s="3" t="s">
         <v>49</v>
       </c>
@@ -3246,7 +3246,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C24" s="3" t="s">
         <v>48</v>
       </c>
@@ -3260,7 +3260,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C25" s="3" t="s">
         <v>47</v>
       </c>
@@ -3274,7 +3274,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>37</v>
       </c>
@@ -3282,12 +3282,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B31" s="2" t="s">
         <v>77</v>
       </c>
@@ -3314,9 +3314,9 @@
       <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3324,7 +3324,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>2</v>
       </c>
@@ -3332,7 +3332,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>35</v>
       </c>
@@ -3340,7 +3340,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>80</v>
       </c>
@@ -3348,7 +3348,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>139</v>
       </c>
@@ -3356,7 +3356,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>200</v>
       </c>
@@ -3364,7 +3364,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>250</v>
       </c>
@@ -3372,7 +3372,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>305</v>
       </c>
@@ -3380,7 +3380,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>396</v>
       </c>
@@ -3388,7 +3388,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>458</v>
       </c>
@@ -3396,7 +3396,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>554</v>
       </c>
@@ -3404,7 +3404,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>591</v>
       </c>
@@ -3412,7 +3412,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>723</v>
       </c>
@@ -3420,7 +3420,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>865</v>
       </c>
@@ -3428,7 +3428,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>1053</v>
       </c>
@@ -3436,7 +3436,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>1149</v>
       </c>
@@ -3444,7 +3444,7 @@
         <v>1017</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>1352</v>
       </c>
@@ -3467,9 +3467,9 @@
       <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3483,7 +3483,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K2">
         <v>0</v>
       </c>
@@ -3491,7 +3491,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K3">
         <v>0</v>
       </c>
@@ -3499,7 +3499,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>62</v>
       </c>
@@ -3513,7 +3513,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>190</v>
       </c>
@@ -3527,7 +3527,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>309</v>
       </c>
@@ -3541,7 +3541,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>414</v>
       </c>
@@ -3555,7 +3555,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>538</v>
       </c>
@@ -3569,7 +3569,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>656</v>
       </c>
@@ -3583,7 +3583,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>768</v>
       </c>
@@ -3597,7 +3597,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>878</v>
       </c>
@@ -3611,7 +3611,7 @@
         <v>808</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1004</v>
       </c>
@@ -3625,7 +3625,7 @@
         <v>904</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1125</v>
       </c>
@@ -3639,7 +3639,7 @@
         <v>998</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1272</v>
       </c>
@@ -3653,7 +3653,7 @@
         <v>1114</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1381</v>
       </c>
@@ -3667,7 +3667,7 @@
         <v>1203</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1491</v>
       </c>
@@ -3681,7 +3681,7 @@
         <v>1284</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1622</v>
       </c>
@@ -3695,7 +3695,7 @@
         <v>1389</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1768</v>
       </c>
@@ -3709,7 +3709,7 @@
         <v>1501</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1870</v>
       </c>
@@ -3723,7 +3723,7 @@
         <v>1583</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1992</v>
       </c>
@@ -3737,7 +3737,7 @@
         <v>1685</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2126</v>
       </c>

</xml_diff>

<commit_message>
fixed pin errors, added battery pin
</commit_message>
<xml_diff>
--- a/pinmap/pinmaps.xlsx
+++ b/pinmap/pinmaps.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FE08CCC-3413-4CB4-9DF2-C9C66431A9B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A003D7C2-2B17-4B41-9E1C-F7A44DDB5CA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5130" yWindow="150" windowWidth="19515" windowHeight="15210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6615" yWindow="690" windowWidth="19515" windowHeight="15210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pinouts" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="94">
   <si>
     <t>ADC</t>
   </si>
@@ -48,9 +48,6 @@
     <t>https://github.com/Xinyuan-LilyGO/TTGO-T-Display</t>
   </si>
   <si>
-    <t>ESP32</t>
-  </si>
-  <si>
     <t>rp2040</t>
   </si>
   <si>
@@ -99,12 +96,6 @@
     <t>IO12</t>
   </si>
   <si>
-    <t>SDA</t>
-  </si>
-  <si>
-    <t>SCL</t>
-  </si>
-  <si>
     <t>3V3</t>
   </si>
   <si>
@@ -277,13 +268,49 @@
   </si>
   <si>
     <t>https://github.com/Xinyuan-LilyGO/LILYGO-T-display-RP2040/blob/main/img/T-display-RP2040.jpg</t>
+  </si>
+  <si>
+    <t>IO0</t>
+  </si>
+  <si>
+    <t>BUTTON0</t>
+  </si>
+  <si>
+    <t>IO35</t>
+  </si>
+  <si>
+    <t>BUTTON1</t>
+  </si>
+  <si>
+    <t>BUTTON_L</t>
+  </si>
+  <si>
+    <t>BUTTON_R</t>
+  </si>
+  <si>
+    <t>IO17</t>
+  </si>
+  <si>
+    <t>IO21</t>
+  </si>
+  <si>
+    <t>esp32c3</t>
+  </si>
+  <si>
+    <t>IO22</t>
+  </si>
+  <si>
+    <t>BATTERY</t>
+  </si>
+  <si>
+    <t>IO34</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -308,6 +335,13 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -367,7 +401,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
@@ -387,6 +421,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2749,560 +2787,622 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD409CAC-30B4-EA46-A79B-63751E99AF2A}">
-  <dimension ref="A1:K31"/>
+  <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+      <selection activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.7109375" customWidth="1"/>
     <col min="2" max="2" width="67.28515625" customWidth="1"/>
-    <col min="3" max="5" width="7.28515625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="7.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="3.28515625" customWidth="1"/>
-    <col min="8" max="8" width="7.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="7.28515625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="8.28515625" customWidth="1"/>
+    <col min="4" max="7" width="8.42578125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="8.42578125" customWidth="1"/>
+    <col min="9" max="12" width="8.42578125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>10</v>
+      <c r="C1" t="s">
+        <v>90</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="J1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>20</v>
+      <c r="C2" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="E2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>27</v>
-      </c>
       <c r="J2" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>20</v>
+        <v>76</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" s="4">
+        <v>19</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="4">
         <v>36</v>
       </c>
-      <c r="I3" s="3" t="s">
-        <v>68</v>
-      </c>
       <c r="J3" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="4">
+        <v>77</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="4">
         <v>21</v>
       </c>
-      <c r="H4" s="4">
+      <c r="I4" s="4">
         <v>37</v>
       </c>
-      <c r="I4" s="3" t="s">
-        <v>69</v>
-      </c>
       <c r="J4" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5" s="4">
+        <v>22</v>
+      </c>
+      <c r="I5" s="4">
+        <v>38</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C6" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="F6" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="4">
+        <v>17</v>
+      </c>
+      <c r="I6" s="4">
+        <v>39</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="4">
+        <v>2</v>
+      </c>
+      <c r="I7" s="4">
+        <v>32</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G8" s="4">
+        <v>15</v>
+      </c>
+      <c r="I8" s="4">
+        <v>33</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G9" s="4">
+        <v>13</v>
+      </c>
+      <c r="I9" s="4">
+        <v>25</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G10" s="4">
+        <v>12</v>
+      </c>
+      <c r="I10" s="4">
         <v>26</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="J10" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I11" s="4">
+        <v>27</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D12" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="L12" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D13" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="K13" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L13" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E14" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G14" s="4">
+        <v>24</v>
+      </c>
+      <c r="I14" s="4"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E15" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G15" s="4">
+        <v>23</v>
+      </c>
+      <c r="I15" s="4"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E16" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G16" s="4">
+        <v>21</v>
+      </c>
+      <c r="I16" s="4"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D18" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I18" t="s">
+        <v>17</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="L18" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D19" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E19" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="G19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" t="s">
+        <v>17</v>
+      </c>
+      <c r="K19" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="L19" s="9" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B21" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="7"/>
+      <c r="D21" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="J21" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K21" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="L21" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D22" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D23" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D24" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D25" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="F5" s="4">
-        <v>22</v>
-      </c>
-      <c r="H5" s="4">
-        <v>38</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D6" s="3" t="s">
+      <c r="E25" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D26" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>34</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C30" s="2"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B31" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E6" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" s="4">
-        <v>17</v>
-      </c>
-      <c r="H6" s="4">
-        <v>39</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F7" s="4">
-        <v>2</v>
-      </c>
-      <c r="H7" s="4">
-        <v>32</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="F8" s="4">
-        <v>15</v>
-      </c>
-      <c r="H8" s="4">
-        <v>33</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C9" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F9" s="4">
-        <v>13</v>
-      </c>
-      <c r="H9" s="4">
-        <v>25</v>
-      </c>
-      <c r="I9" s="3" t="s">
+      <c r="C31" s="2"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B32" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="J9" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C10" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F10" s="4">
-        <v>12</v>
-      </c>
-      <c r="H10" s="4">
-        <v>26</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="K10" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C11" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H11" s="4">
-        <v>27</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="J11" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="K11" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C12" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="I12" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="J12" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="K12" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C13" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="I13" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="J13" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="K13" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D14" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="F14" s="4">
-        <v>24</v>
-      </c>
-      <c r="H14" s="4"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D15" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="F15" s="4">
-        <v>23</v>
-      </c>
-      <c r="H15" s="4"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D16" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="F16" s="4">
-        <v>21</v>
-      </c>
-      <c r="H16" s="4"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C18" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H18" t="s">
-        <v>18</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="J18" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B20" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C21" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C22" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C23" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C24" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C25" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>37</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B30" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B31" s="2" t="s">
-        <v>77</v>
-      </c>
+      <c r="C32" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{538BA5B6-7DAF-BF46-9D75-F1CD68024CC7}"/>
     <hyperlink ref="B4" r:id="rId2" xr:uid="{6CC79B36-DDED-BC4A-B925-767D303582FE}"/>
-    <hyperlink ref="B29" r:id="rId3" xr:uid="{EF86182E-42C0-5141-A896-71BDC0841FFA}"/>
-    <hyperlink ref="B31" r:id="rId4" xr:uid="{4A7544E9-DDF2-4645-889B-9BD581E6F4D4}"/>
+    <hyperlink ref="B30" r:id="rId3" xr:uid="{EF86182E-42C0-5141-A896-71BDC0841FFA}"/>
+    <hyperlink ref="B32" r:id="rId4" xr:uid="{4A7544E9-DDF2-4645-889B-9BD581E6F4D4}"/>
     <hyperlink ref="B5" r:id="rId5" xr:uid="{DCC43695-1A22-BB4B-A4B8-3D512BB8363E}"/>
     <hyperlink ref="B3" r:id="rId6" xr:uid="{796CA9F0-001E-0A4B-830C-1358E1CEA9C9}"/>
-    <hyperlink ref="B30" r:id="rId7" xr:uid="{B3813BBD-D388-B946-9DFD-A7EFFB599401}"/>
+    <hyperlink ref="B31" r:id="rId7" xr:uid="{B3813BBD-D388-B946-9DFD-A7EFFB599401}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
 

</xml_diff>